<commit_message>
- Updated documentation. - Minor refactoring in depdencies and source code.
</commit_message>
<xml_diff>
--- a/docs/source/_static/xlsx_example.xlsx
+++ b/docs/source/_static/xlsx_example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="495"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28260" tabRatio="495"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="186">
   <si>
     <t>begin group</t>
   </si>
@@ -512,73 +512,85 @@
     <t>Joe</t>
   </si>
   <si>
+    <t>2018-06-10 &lt;&gt; 2019-06-10</t>
+  </si>
+  <si>
+    <t>today() &lt; date("2018-06-10") or today() &gt; date("2019-06-10")</t>
+  </si>
+  <si>
+    <t>today() &gt; date("2018-06-10") and today() &lt; date("2019-06-10")</t>
+  </si>
+  <si>
+    <t>. &gt; date("2018-06-10") and . &lt; date("2019-06-10")</t>
+  </si>
+  <si>
+    <t>${system_date_check} = 'no' or today() &lt; date("2018-06-10") or today() &gt; date("2019-06-10")</t>
+  </si>
+  <si>
+    <t>EA_location_a</t>
+  </si>
+  <si>
+    <t>EA_location_b</t>
+  </si>
+  <si>
+    <t>EA_location_c</t>
+  </si>
+  <si>
+    <t>EA_location_d</t>
+  </si>
+  <si>
+    <t>EA_location_e</t>
+  </si>
+  <si>
+    <t>EA a</t>
+  </si>
+  <si>
+    <t>EA b</t>
+  </si>
+  <si>
+    <t>EA c</t>
+  </si>
+  <si>
+    <t>EA d</t>
+  </si>
+  <si>
+    <t>EA e</t>
+  </si>
+  <si>
+    <t>[252, 777]</t>
+  </si>
+  <si>
+    <t>[123, 999]</t>
+  </si>
+  <si>
+    <t>[636, 444]</t>
+  </si>
+  <si>
+    <t>[252: 123-636&amp;#x0a;, 777: 999-444&amp;#x0a;]</t>
+  </si>
+  <si>
+    <t>252: 123-636&amp;#x0a;777: 999-444&amp;#x0a;</t>
+  </si>
+  <si>
+    <t>bind::xtest-linearAssert</t>
+  </si>
+  <si>
+    <t>relevant: 1</t>
+  </si>
+  <si>
+    <t>relevant: 0</t>
+  </si>
+  <si>
+    <t>string-length(.) &lt;= 15</t>
+  </si>
+  <si>
     <t>{relevant: 0}</t>
   </si>
   <si>
-    <t>{relevant: 1}</t>
-  </si>
-  <si>
-    <t>2018-06-10 &lt;&gt; 2019-06-10</t>
-  </si>
-  <si>
-    <t>today() &lt; date("2018-06-10") or today() &gt; date("2019-06-10")</t>
-  </si>
-  <si>
-    <t>today() &gt; date("2018-06-10") and today() &lt; date("2019-06-10")</t>
-  </si>
-  <si>
-    <t>. &gt; date("2018-06-10") and . &lt; date("2019-06-10")</t>
-  </si>
-  <si>
-    <t>${system_date_check} = 'no' or today() &lt; date("2018-06-10") or today() &gt; date("2019-06-10")</t>
-  </si>
-  <si>
-    <t>EA_location_a</t>
-  </si>
-  <si>
-    <t>EA_location_b</t>
-  </si>
-  <si>
-    <t>EA_location_c</t>
-  </si>
-  <si>
-    <t>EA_location_d</t>
-  </si>
-  <si>
-    <t>EA_location_e</t>
-  </si>
-  <si>
-    <t>EA a</t>
-  </si>
-  <si>
-    <t>EA b</t>
-  </si>
-  <si>
-    <t>EA c</t>
-  </si>
-  <si>
-    <t>EA d</t>
-  </si>
-  <si>
-    <t>EA e</t>
-  </si>
-  <si>
-    <t>[252, 777]</t>
-  </si>
-  <si>
-    <t>[123, 999]</t>
-  </si>
-  <si>
-    <t>[636, 444]</t>
-  </si>
-  <si>
-    <t>[252: 123-636&amp;#x0a;, 777: 999-444&amp;#x0a;]</t>
-  </si>
-  <si>
-    <t>252: 123-636&amp;#x0a;777: 999-444&amp;#x0a;</t>
-  </si>
-  <si>
-    <t>bind::xtest-linearAssert</t>
+    <t>relevant: 1, value: Joe, constraint: null</t>
+  </si>
+  <si>
+    <t>value: Country, relevant: 1</t>
   </si>
 </sst>
 </file>
@@ -664,11 +676,317 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -861,7 +1179,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="152">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -886,6 +1204,57 @@
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -910,6 +1279,57 @@
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2" xfId="1"/>
   </cellStyles>
@@ -1360,11 +1780,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -1376,11 +1796,11 @@
     <col min="5" max="5" width="8.5" style="1" customWidth="1"/>
     <col min="6" max="8" width="3.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="3.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5" style="1" customWidth="1"/>
     <col min="11" max="11" width="4" style="1" customWidth="1"/>
     <col min="12" max="12" width="9.6640625" style="1"/>
     <col min="13" max="13" width="5.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="34.33203125" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9.6640625" style="1"/>
   </cols>
   <sheetData>
@@ -1425,7 +1845,7 @@
         <v>61</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="13" customHeight="1">
@@ -1439,16 +1859,16 @@
         <v>111</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="13" customHeight="1">
@@ -1465,7 +1885,7 @@
         <v>112</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="13" customHeight="1">
@@ -1485,7 +1905,7 @@
         <v>114</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="13" customHeight="1">
@@ -1501,6 +1921,9 @@
       <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1508,7 +1931,7 @@
         <v>115</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>158</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="13" customHeight="1">
@@ -1522,10 +1945,10 @@
         <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="13" customHeight="1">
@@ -1546,7 +1969,7 @@
       </c>
       <c r="N7" s="13">
         <f ca="1">TODAY()</f>
-        <v>43308</v>
+        <v>43391</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="13" customHeight="1">
@@ -1574,7 +1997,7 @@
         <v>29</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="13" customHeight="1">
@@ -1588,10 +2011,10 @@
         <v>117</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>13</v>
@@ -1600,10 +2023,10 @@
         <v>116</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="4" customFormat="1" ht="13" customHeight="1">
@@ -1627,7 +2050,7 @@
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="12" t="s">
-        <v>144</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="4" customFormat="1" ht="13" customHeight="1">
@@ -1717,7 +2140,7 @@
         <v>132</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="13" customHeight="1">
@@ -1749,7 +2172,7 @@
       </c>
       <c r="M16" s="5"/>
       <c r="N16" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="13" customHeight="1">
@@ -1763,7 +2186,7 @@
         <v>44</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="13" customHeight="1">
@@ -1778,7 +2201,7 @@
         <v>1</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="13" customHeight="1">
@@ -1795,7 +2218,7 @@
         <v>13</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="13" customHeight="1">
@@ -1812,7 +2235,7 @@
         <v>13</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="13" customHeight="1">
@@ -1829,7 +2252,7 @@
         <v>13</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="13" customHeight="1">
@@ -1841,7 +2264,7 @@
       </c>
       <c r="C22" s="6"/>
       <c r="N22" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="13" customHeight="1">
@@ -1856,7 +2279,7 @@
         <v>75</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="13" customHeight="1">
@@ -1868,7 +2291,7 @@
       </c>
       <c r="C24" s="6"/>
       <c r="N24" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="13" customHeight="1">
@@ -1910,7 +2333,7 @@
         <v>86</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="13" customHeight="1">
@@ -1924,7 +2347,7 @@
         <v>1</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="13" customHeight="1">
@@ -1938,7 +2361,7 @@
         <v>78</v>
       </c>
       <c r="N29" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="13" customHeight="1">
@@ -1966,7 +2389,7 @@
         <v>87</v>
       </c>
       <c r="N31" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="13" customHeight="1">
@@ -1986,7 +2409,7 @@
         <v>90</v>
       </c>
       <c r="N32" s="12" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="13" customHeight="1">
@@ -2046,7 +2469,7 @@
         <v>80</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="13" customHeight="1">
@@ -2066,7 +2489,7 @@
         <v>56</v>
       </c>
       <c r="N36" s="12" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="13" customHeight="1">
@@ -2083,7 +2506,7 @@
         <v>101</v>
       </c>
       <c r="N37" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="13" customHeight="1">
@@ -2191,7 +2614,7 @@
       <c r="D42" s="4"/>
       <c r="F42" s="4"/>
       <c r="N42" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:14" s="5" customFormat="1" ht="13" customHeight="1">
@@ -2207,7 +2630,7 @@
       <c r="D43" s="4"/>
       <c r="F43" s="4"/>
       <c r="N43" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:14" s="5" customFormat="1" ht="13" customHeight="1">
@@ -2223,7 +2646,7 @@
       <c r="D44" s="4"/>
       <c r="F44" s="4"/>
       <c r="N44" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:14" s="5" customFormat="1" ht="13" customHeight="1">
@@ -2239,7 +2662,7 @@
       <c r="D45" s="4"/>
       <c r="F45" s="4"/>
       <c r="N45" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:14" s="5" customFormat="1" ht="13" customHeight="1">
@@ -2255,7 +2678,7 @@
       <c r="D46" s="4"/>
       <c r="F46" s="4"/>
       <c r="N46" s="12" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="3:3" ht="13" customHeight="1">
@@ -2522,10 +2945,10 @@
         <v>102</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>153</v>
@@ -2536,10 +2959,10 @@
         <v>102</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>154</v>
@@ -2550,10 +2973,10 @@
         <v>102</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>155</v>
@@ -2564,10 +2987,10 @@
         <v>102</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>156</v>
@@ -2578,10 +3001,10 @@
         <v>102</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>157</v>

</xml_diff>